<commit_message>
Commit the New Line of codes
</commit_message>
<xml_diff>
--- a/AllTeachersPortalAutomation/TestData/AllTeacherTestDatas.xlsx
+++ b/AllTeachersPortalAutomation/TestData/AllTeacherTestDatas.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1886f220f6a057ee/Desktop/Desktop Items/AllTeacher/AllTeacherAutomation/AllTeachersPortalAutomation/TestData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hp\git\AllTeacher-Selenium-Automation\AllTeachersPortalAutomation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{E66D4AE4-D174-498F-9684-D99F9F60FEB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1E397A62-87F9-43A9-8AC7-0CB5CA9B53EB}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21007F0C-43BB-4FCE-BC2F-6012330EA765}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="8" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -25,18 +25,32 @@
     <sheet name="Languages" sheetId="10" r:id="rId10"/>
     <sheet name="Students" sheetId="11" r:id="rId11"/>
     <sheet name="ChatBot" sheetId="12" r:id="rId12"/>
+    <sheet name="DiscoveryContent" sheetId="13" r:id="rId13"/>
+    <sheet name="Sheet3" sheetId="14" r:id="rId14"/>
+    <sheet name="Sheet4" sheetId="15" r:id="rId15"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1034" uniqueCount="233">
   <si>
     <t>Username</t>
   </si>
@@ -548,12 +562,282 @@
   <si>
     <t>Validating Viewing On Cohort</t>
   </si>
+  <si>
+    <t>Validate on Discovery Content Feature on Class III</t>
+  </si>
+  <si>
+    <t>Validate on Discovery Content Feature on Class I</t>
+  </si>
+  <si>
+    <t>Validate on Discovery Content Feature on Class II</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weigh man </t>
+  </si>
+  <si>
+    <t>GRN No</t>
+  </si>
+  <si>
+    <t>FRJ NO</t>
+  </si>
+  <si>
+    <t>Type of Cofee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grade </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quantity </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Purchase Order </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suppler ID &amp; Name </t>
+  </si>
+  <si>
+    <t>Type of coffee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Price </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bags </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1st of Creation </t>
+  </si>
+  <si>
+    <t>Manage PO</t>
+  </si>
+  <si>
+    <t>RAW</t>
+  </si>
+  <si>
+    <t>AAA</t>
+  </si>
+  <si>
+    <t>PO_001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Robin </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRN </t>
+  </si>
+  <si>
+    <t>Supp,ier ID</t>
+  </si>
+  <si>
+    <t>AR001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual Quanity </t>
+  </si>
+  <si>
+    <t>GRN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Balance </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Save &amp; submit </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Close </t>
+  </si>
+  <si>
+    <t>close the PO</t>
+  </si>
+  <si>
+    <t>Close PO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Load Number </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRN Number </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Form J Number </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date </t>
+  </si>
+  <si>
+    <t>Type of Coffee</t>
+  </si>
+  <si>
+    <t>Grade</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stored IN </t>
+  </si>
+  <si>
+    <t>Farmer / Supplier Name</t>
+  </si>
+  <si>
+    <t>Vechile No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Other fields </t>
+  </si>
+  <si>
+    <t>Driver Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Loaders </t>
+  </si>
+  <si>
+    <t>Unloaders</t>
+  </si>
+  <si>
+    <t>D27</t>
+  </si>
+  <si>
+    <t>FRJ001</t>
+  </si>
+  <si>
+    <t>Robusta Cherry (RC)</t>
+  </si>
+  <si>
+    <t>Unit 1</t>
+  </si>
+  <si>
+    <t>Buffy Caldwell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Farmer / Supplier </t>
+  </si>
+  <si>
+    <t>SU0028</t>
+  </si>
+  <si>
+    <t>&gt;</t>
+  </si>
+  <si>
+    <t>PO110824001</t>
+  </si>
+  <si>
+    <t>Buffy Caldwell &amp; SU0028</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Price per Bag </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arriving load Details </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Created Yesterday </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Today Arrived </t>
+  </si>
+  <si>
+    <t>Actions (3 Actions are Icons only )</t>
+  </si>
+  <si>
+    <t>View   Edit  Connect GRN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add New Record  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mapping One </t>
+  </si>
+  <si>
+    <t>GRN Number(DropDown Values )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">After Proceed Quantity </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Remaining Quantity </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Purchase Order Details </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Got Idea of Creating this In Pop-up </t>
+  </si>
+  <si>
+    <t>AR0056</t>
+  </si>
+  <si>
+    <t>AR0082</t>
+  </si>
+  <si>
+    <t>AR0083</t>
+  </si>
+  <si>
+    <t>AR0084</t>
+  </si>
+  <si>
+    <t>AR0085</t>
+  </si>
+  <si>
+    <t>AR0086</t>
+  </si>
+  <si>
+    <t>13/2/2025</t>
+  </si>
+  <si>
+    <t>When the remaining fields comes as 0.</t>
+  </si>
+  <si>
+    <t>Actions (This has to turn to view &amp; Status )</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">View  , Status PO </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Closed </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">By Manager </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mapping Two </t>
+  </si>
+  <si>
+    <t>Mapping Three</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mapping Four </t>
+  </si>
+  <si>
+    <t>Mapping Five</t>
+  </si>
+  <si>
+    <t>Mapping Six</t>
+  </si>
+  <si>
+    <t>Mapping Seven</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When I Click New Record A Pop Up should display </t>
+  </si>
+  <si>
+    <t>After Closing the PO the table will be:</t>
+  </si>
+  <si>
+    <t>When the remaining comes as 0. Close PO</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -593,16 +877,65 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -658,12 +991,25 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -679,6 +1025,20 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2108,6 +2468,2147 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A2F4C80-D325-475E-B243-6584F08EE0B4}">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="42.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.08984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.6328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{157309FB-C423-47A9-9E10-275D1A073638}">
+  <dimension ref="A1:Q102"/>
+  <sheetViews>
+    <sheetView topLeftCell="M86" workbookViewId="0">
+      <selection activeCell="O96" sqref="O96"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="2" max="2" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="32" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.90625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="43.08984375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="33.36328125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="36.36328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:15">
+      <c r="J1" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="K1" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="L1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="2" spans="2:15">
+      <c r="F2" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="J2" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="K2" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="L2" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="M2" s="16" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="3" spans="2:15">
+      <c r="J3" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15">
+      <c r="E4" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="F4" t="s">
+        <v>165</v>
+      </c>
+      <c r="J4" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="K4" s="16" t="s">
+        <v>200</v>
+      </c>
+      <c r="L4" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="M4" s="16" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15">
+      <c r="E5" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="F5" t="s">
+        <v>166</v>
+      </c>
+      <c r="J5" s="1">
+        <v>1000</v>
+      </c>
+      <c r="K5" s="1">
+        <v>2500</v>
+      </c>
+      <c r="L5" s="1">
+        <v>25</v>
+      </c>
+      <c r="M5" s="15">
+        <v>45604</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15">
+      <c r="E6" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="F6" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15">
+      <c r="E7" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="F7" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15">
+      <c r="E8" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="F8">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15">
+      <c r="E9" s="13" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15">
+      <c r="E10" s="13" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15">
+      <c r="B12" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="J12" s="17" t="s">
+        <v>201</v>
+      </c>
+      <c r="K12" s="17" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15">
+      <c r="B13" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="C13" t="s">
+        <v>169</v>
+      </c>
+      <c r="J13" s="16" t="s">
+        <v>177</v>
+      </c>
+      <c r="K13" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="L13" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="M13" s="16" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15">
+      <c r="B14" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="C14" t="s">
+        <v>166</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="M14" s="15">
+        <v>45605</v>
+      </c>
+      <c r="O14" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15">
+      <c r="B15" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="C15" t="s">
+        <v>163</v>
+      </c>
+      <c r="J15" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="K15" s="16" t="s">
+        <v>182</v>
+      </c>
+      <c r="L15" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="M15" s="1"/>
+      <c r="N15" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="O15" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15">
+      <c r="B16" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="C16" t="s">
+        <v>164</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="L16" s="1">
+        <v>50</v>
+      </c>
+      <c r="M16" s="1"/>
+      <c r="O16" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="17" spans="2:17">
+      <c r="B17" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="C17">
+        <v>20</v>
+      </c>
+      <c r="J17" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="K17" s="16" t="s">
+        <v>183</v>
+      </c>
+      <c r="L17" s="16" t="s">
+        <v>184</v>
+      </c>
+      <c r="M17" s="16" t="s">
+        <v>195</v>
+      </c>
+      <c r="O17" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="18" spans="2:17">
+      <c r="B18" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="J18" s="1">
+        <v>25</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="O18" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="19" spans="2:17">
+      <c r="G19" s="14" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="21" spans="2:17">
+      <c r="F21" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="G21" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="22" spans="2:17">
+      <c r="C22">
+        <v>30</v>
+      </c>
+      <c r="F22" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="G22" t="s">
+        <v>166</v>
+      </c>
+      <c r="J22" s="18" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="23" spans="2:17">
+      <c r="F23" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="G23" t="s">
+        <v>163</v>
+      </c>
+      <c r="J23" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="K23" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="L23" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="M23" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="N23" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="O23" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="P23" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q23" s="16" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="24" spans="2:17">
+      <c r="F24" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="G24" t="s">
+        <v>164</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="N24" s="1">
+        <v>1000</v>
+      </c>
+      <c r="O24" s="1">
+        <v>2500</v>
+      </c>
+      <c r="P24" s="1">
+        <v>25</v>
+      </c>
+      <c r="Q24" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="25" spans="2:17">
+      <c r="F25" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="G25">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="26" spans="2:17">
+      <c r="F26" s="13" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="27" spans="2:17">
+      <c r="F27" s="13" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="29" spans="2:17">
+      <c r="M29" s="20"/>
+    </row>
+    <row r="31" spans="2:17">
+      <c r="J31" s="18"/>
+    </row>
+    <row r="32" spans="2:17">
+      <c r="J32" s="16"/>
+      <c r="K32" s="16"/>
+      <c r="L32" s="16"/>
+      <c r="M32" s="16"/>
+    </row>
+    <row r="33" spans="1:16">
+      <c r="J33" s="1"/>
+      <c r="K33" s="1"/>
+      <c r="L33" s="1"/>
+      <c r="M33" s="1"/>
+    </row>
+    <row r="34" spans="1:16">
+      <c r="J34" s="16"/>
+      <c r="K34" s="16"/>
+      <c r="L34" s="16"/>
+      <c r="M34" s="16"/>
+    </row>
+    <row r="35" spans="1:16">
+      <c r="J35" s="1"/>
+      <c r="K35" s="1"/>
+      <c r="L35" s="1"/>
+      <c r="M35" s="15"/>
+    </row>
+    <row r="38" spans="1:16">
+      <c r="P38" s="22" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16">
+      <c r="J39" s="17"/>
+    </row>
+    <row r="40" spans="1:16">
+      <c r="J40" s="16"/>
+      <c r="K40" s="16"/>
+      <c r="L40" s="16"/>
+      <c r="M40" s="16"/>
+      <c r="N40" s="16" t="s">
+        <v>209</v>
+      </c>
+      <c r="O40" s="16" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16">
+      <c r="J41" s="1"/>
+      <c r="K41" s="1"/>
+      <c r="L41" s="15"/>
+      <c r="M41" s="1"/>
+      <c r="N41" s="1">
+        <v>30</v>
+      </c>
+      <c r="O41" s="1">
+        <f>(M41-N41)</f>
+        <v>-30</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16">
+      <c r="J42" s="1"/>
+      <c r="K42" s="1"/>
+      <c r="L42" s="15"/>
+      <c r="M42" s="1"/>
+      <c r="N42" s="1">
+        <v>300</v>
+      </c>
+      <c r="O42" s="1">
+        <f>(M42-N42)</f>
+        <v>-300</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16">
+      <c r="J43" s="1"/>
+      <c r="K43" s="1"/>
+      <c r="L43" s="21"/>
+      <c r="M43" s="1"/>
+      <c r="N43" s="1">
+        <v>200</v>
+      </c>
+      <c r="O43" s="1">
+        <f>(M43-N43)</f>
+        <v>-200</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16">
+      <c r="A44" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J44" s="1"/>
+      <c r="K44" s="1"/>
+      <c r="L44" s="15"/>
+      <c r="M44" s="1"/>
+      <c r="N44" s="1">
+        <v>300</v>
+      </c>
+      <c r="O44" s="1">
+        <f>(M44-N44)</f>
+        <v>-300</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16">
+      <c r="A45" s="1"/>
+      <c r="B45" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C45" s="1">
+        <v>1000</v>
+      </c>
+      <c r="D45" s="1">
+        <v>20</v>
+      </c>
+      <c r="E45" s="1">
+        <v>980</v>
+      </c>
+      <c r="J45" s="1"/>
+      <c r="K45" s="1"/>
+      <c r="L45" s="15"/>
+      <c r="M45" s="1"/>
+      <c r="N45" s="1">
+        <v>70</v>
+      </c>
+      <c r="O45" s="1">
+        <f>(M45-N45)</f>
+        <v>-70</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16">
+      <c r="A46" s="1"/>
+      <c r="B46" s="1"/>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+      <c r="J46" s="1"/>
+      <c r="K46" s="1"/>
+      <c r="L46" s="21"/>
+      <c r="M46" s="1"/>
+      <c r="N46" s="1">
+        <v>30</v>
+      </c>
+      <c r="O46" s="1">
+        <f>(M46-N46)</f>
+        <v>-30</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16">
+      <c r="A47" s="1"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+      <c r="F47" t="s">
+        <v>173</v>
+      </c>
+      <c r="J47" s="1"/>
+      <c r="K47" s="1"/>
+      <c r="L47" s="23"/>
+      <c r="M47" s="1"/>
+      <c r="N47" s="1">
+        <v>40</v>
+      </c>
+      <c r="O47" s="1">
+        <f>(M47-N47)</f>
+        <v>-40</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16">
+      <c r="A48" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B48" s="1"/>
+      <c r="C48" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="O48" s="8"/>
+    </row>
+    <row r="49" spans="1:16">
+      <c r="A49" s="1"/>
+      <c r="B49" s="1"/>
+      <c r="C49" s="1">
+        <v>980</v>
+      </c>
+      <c r="D49" s="1">
+        <v>30</v>
+      </c>
+      <c r="E49" s="1">
+        <v>950</v>
+      </c>
+      <c r="P49" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16">
+      <c r="A50" s="1"/>
+      <c r="B50" s="1"/>
+      <c r="C50" s="1"/>
+      <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
+      <c r="F50" t="s">
+        <v>174</v>
+      </c>
+      <c r="P50" s="17" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16">
+      <c r="A51" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B51" s="1"/>
+      <c r="C51" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16">
+      <c r="A52" s="1"/>
+      <c r="B52" s="1"/>
+      <c r="C52" s="1">
+        <v>1000</v>
+      </c>
+      <c r="D52" s="1">
+        <v>20</v>
+      </c>
+      <c r="E52" s="1">
+        <v>980</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16">
+      <c r="A53" s="1"/>
+      <c r="B53" s="1"/>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1"/>
+      <c r="E53" s="1"/>
+    </row>
+    <row r="54" spans="1:16">
+      <c r="A54" s="1"/>
+      <c r="B54" s="1"/>
+      <c r="C54" s="1"/>
+      <c r="D54" s="1"/>
+      <c r="E54" s="1"/>
+    </row>
+    <row r="55" spans="1:16">
+      <c r="A55" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B55" s="1"/>
+      <c r="C55" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16">
+      <c r="A56" s="1"/>
+      <c r="B56" s="1"/>
+      <c r="C56" s="1">
+        <v>980</v>
+      </c>
+      <c r="D56" s="1">
+        <v>30</v>
+      </c>
+      <c r="E56" s="1">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16">
+      <c r="A57" s="1"/>
+      <c r="B57" s="1"/>
+      <c r="C57" s="1"/>
+      <c r="D57" s="1"/>
+      <c r="E57" s="1"/>
+    </row>
+    <row r="58" spans="1:16">
+      <c r="A58" s="1"/>
+      <c r="B58" s="1"/>
+      <c r="C58" s="1"/>
+      <c r="D58" s="1"/>
+      <c r="E58" s="1"/>
+    </row>
+    <row r="59" spans="1:16">
+      <c r="A59" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B59" s="1"/>
+      <c r="C59" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16">
+      <c r="A60" s="1"/>
+      <c r="B60" s="1"/>
+      <c r="C60" s="1">
+        <v>1000</v>
+      </c>
+      <c r="D60" s="1">
+        <v>20</v>
+      </c>
+      <c r="E60" s="1">
+        <v>980</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16">
+      <c r="A61" s="1"/>
+      <c r="B61" s="1"/>
+      <c r="C61" s="1"/>
+      <c r="D61" s="1"/>
+      <c r="E61" s="1"/>
+    </row>
+    <row r="62" spans="1:16">
+      <c r="A62" s="1"/>
+      <c r="B62" s="1"/>
+      <c r="C62" s="1"/>
+      <c r="D62" s="1"/>
+      <c r="E62" s="1"/>
+      <c r="M62" s="20" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16">
+      <c r="A63" s="1"/>
+      <c r="B63" s="1"/>
+      <c r="C63" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16">
+      <c r="A64" s="1"/>
+      <c r="B64" s="1"/>
+      <c r="C64" s="1">
+        <v>980</v>
+      </c>
+      <c r="D64" s="1">
+        <v>30</v>
+      </c>
+      <c r="E64" s="1">
+        <v>950</v>
+      </c>
+      <c r="J64" s="18" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15">
+      <c r="A65" s="1"/>
+      <c r="B65" s="1"/>
+      <c r="C65" s="1"/>
+      <c r="D65" s="1"/>
+      <c r="E65" s="1"/>
+      <c r="J65" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="K65" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="L65" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="M65" s="16" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15">
+      <c r="A66" s="1"/>
+      <c r="B66" s="1"/>
+      <c r="C66" s="1"/>
+      <c r="D66" s="1"/>
+      <c r="E66" s="1">
+        <v>0</v>
+      </c>
+      <c r="J66" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="K66" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="L66" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="M66" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15">
+      <c r="F67" t="s">
+        <v>175</v>
+      </c>
+      <c r="J67" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="K67" s="16" t="s">
+        <v>200</v>
+      </c>
+      <c r="L67" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="M67" s="16" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15">
+      <c r="J68" s="1">
+        <v>1000</v>
+      </c>
+      <c r="K68" s="1">
+        <v>2500</v>
+      </c>
+      <c r="L68" s="1">
+        <v>25</v>
+      </c>
+      <c r="M68" s="15">
+        <v>45604</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15">
+      <c r="O69" s="20" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15">
+      <c r="J70" s="17" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15">
+      <c r="J71" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="K71" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="L71" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="M71" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="N71" s="16" t="s">
+        <v>209</v>
+      </c>
+      <c r="O71" s="16" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="72" spans="1:15">
+      <c r="J72" s="1"/>
+      <c r="K72" s="1"/>
+      <c r="L72" s="15"/>
+      <c r="M72" s="1"/>
+      <c r="N72" s="1"/>
+      <c r="O72" s="1"/>
+    </row>
+    <row r="76" spans="1:15">
+      <c r="J76" s="17" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="77" spans="1:15">
+      <c r="J77" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="K77" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="L77" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="M77" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="N77" s="16" t="s">
+        <v>209</v>
+      </c>
+      <c r="O77" s="16" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="78" spans="1:15">
+      <c r="J78" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="K78" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="L78" s="15">
+        <v>45604</v>
+      </c>
+      <c r="M78" s="1">
+        <v>1000</v>
+      </c>
+      <c r="N78" s="1">
+        <v>30</v>
+      </c>
+      <c r="O78" s="1">
+        <f>(M78-N78)</f>
+        <v>970</v>
+      </c>
+    </row>
+    <row r="79" spans="1:15">
+      <c r="J79" s="17" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="80" spans="1:15">
+      <c r="J80" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="K80" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="L80" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="M80" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="N80" s="16" t="s">
+        <v>209</v>
+      </c>
+      <c r="O80" s="16" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="81" spans="10:15">
+      <c r="J81" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="K81" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="L81" s="15">
+        <v>45634</v>
+      </c>
+      <c r="M81" s="1">
+        <v>970</v>
+      </c>
+      <c r="N81" s="1">
+        <v>300</v>
+      </c>
+      <c r="O81" s="1">
+        <f>(M81-N81)</f>
+        <v>670</v>
+      </c>
+    </row>
+    <row r="82" spans="10:15">
+      <c r="J82" s="17" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="83" spans="10:15">
+      <c r="J83" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="K83" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="L83" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="M83" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="N83" s="16" t="s">
+        <v>209</v>
+      </c>
+      <c r="O83" s="16" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="84" spans="10:15">
+      <c r="J84" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="K84" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="L84" s="21">
+        <v>45682</v>
+      </c>
+      <c r="M84" s="1">
+        <v>670</v>
+      </c>
+      <c r="N84" s="1">
+        <v>200</v>
+      </c>
+      <c r="O84" s="1">
+        <f>(M84-N84)</f>
+        <v>470</v>
+      </c>
+    </row>
+    <row r="85" spans="10:15">
+      <c r="J85" s="17" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="86" spans="10:15">
+      <c r="J86" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="K86" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="L86" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="M86" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="N86" s="16" t="s">
+        <v>209</v>
+      </c>
+      <c r="O86" s="16" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="87" spans="10:15">
+      <c r="J87" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="K87" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="L87" s="15">
+        <v>45690</v>
+      </c>
+      <c r="M87" s="1">
+        <v>470</v>
+      </c>
+      <c r="N87" s="1">
+        <v>300</v>
+      </c>
+      <c r="O87" s="1">
+        <f>(M87-N87)</f>
+        <v>170</v>
+      </c>
+    </row>
+    <row r="88" spans="10:15">
+      <c r="J88" s="17" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="89" spans="10:15">
+      <c r="J89" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="K89" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="L89" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="M89" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="N89" s="16" t="s">
+        <v>209</v>
+      </c>
+      <c r="O89" s="16" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="90" spans="10:15">
+      <c r="J90" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="K90" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="L90" s="15">
+        <v>45779</v>
+      </c>
+      <c r="M90" s="1">
+        <v>170</v>
+      </c>
+      <c r="N90" s="1">
+        <v>70</v>
+      </c>
+      <c r="O90" s="1">
+        <f>(M90-N90)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="91" spans="10:15">
+      <c r="J91" s="17" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="92" spans="10:15">
+      <c r="J92" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="K92" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="L92" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="M92" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="N92" s="16" t="s">
+        <v>209</v>
+      </c>
+      <c r="O92" s="16" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="93" spans="10:15">
+      <c r="J93" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="K93" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="L93" s="21">
+        <v>45932</v>
+      </c>
+      <c r="M93" s="1">
+        <v>70</v>
+      </c>
+      <c r="N93" s="1">
+        <v>30</v>
+      </c>
+      <c r="O93" s="1">
+        <f>(M93-N93)</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="94" spans="10:15">
+      <c r="J94" s="17" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="95" spans="10:15">
+      <c r="J95" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="K95" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="L95" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="M95" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="N95" s="16" t="s">
+        <v>209</v>
+      </c>
+      <c r="O95" s="16" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="96" spans="10:15">
+      <c r="J96" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="K96" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="L96" s="23" t="s">
+        <v>219</v>
+      </c>
+      <c r="M96" s="1">
+        <v>40</v>
+      </c>
+      <c r="N96" s="1">
+        <v>40</v>
+      </c>
+      <c r="O96" s="1">
+        <f>(M96-N96)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="10:17">
+      <c r="J99" s="19" t="s">
+        <v>231</v>
+      </c>
+      <c r="O99" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="100" spans="10:17">
+      <c r="J100" s="18" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="101" spans="10:17">
+      <c r="J101" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="K101" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="L101" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="M101" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="N101" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="O101" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="P101" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q101" s="16" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="102" spans="10:17">
+      <c r="J102" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="K102" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="L102" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="M102" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="N102" s="1">
+        <v>1000</v>
+      </c>
+      <c r="O102" s="1">
+        <v>2500</v>
+      </c>
+      <c r="P102" s="1">
+        <v>25</v>
+      </c>
+      <c r="Q102" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11CA283F-9A2E-44C4-A5E9-4BA2FD0ECCBB}">
+  <dimension ref="A1:H63"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="F60" sqref="F60"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="43.08984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="C1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>200</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1">
+        <v>1000</v>
+      </c>
+      <c r="B5" s="1">
+        <v>2500</v>
+      </c>
+      <c r="C5" s="1">
+        <v>25</v>
+      </c>
+      <c r="D5" s="15">
+        <v>45604</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="17" t="s">
+        <v>201</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="16" t="s">
+        <v>177</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="D10" s="15">
+        <v>45605</v>
+      </c>
+      <c r="F10" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>182</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="F11" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C12" s="1">
+        <v>50</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="F12" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>183</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>184</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>195</v>
+      </c>
+      <c r="F13" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="1">
+        <v>25</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="18" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="E19" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="F19" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="G19" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="H19" s="16" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="E20" s="1">
+        <v>1000</v>
+      </c>
+      <c r="F20" s="1">
+        <v>2500</v>
+      </c>
+      <c r="G20" s="1">
+        <v>25</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="D23" s="20" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="18" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="B26" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="C26" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="D26" s="16" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="B28" s="16" t="s">
+        <v>200</v>
+      </c>
+      <c r="C28" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="D28" s="16" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" s="1">
+        <v>1000</v>
+      </c>
+      <c r="B29" s="1">
+        <v>2500</v>
+      </c>
+      <c r="C29" s="1">
+        <v>25</v>
+      </c>
+      <c r="D29" s="15">
+        <v>45604</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="F30" s="20" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" s="17" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="B32" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="C32" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="D32" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="E32" s="16" t="s">
+        <v>209</v>
+      </c>
+      <c r="F32" s="16" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" s="17" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="B38" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="C38" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="D38" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="E38" s="16" t="s">
+        <v>209</v>
+      </c>
+      <c r="F38" s="16" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C39" s="15">
+        <v>45604</v>
+      </c>
+      <c r="D39" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E39" s="1">
+        <v>30</v>
+      </c>
+      <c r="F39" s="1">
+        <f>(D39-E39)</f>
+        <v>970</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" s="17" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="B41" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="C41" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="D41" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="E41" s="16" t="s">
+        <v>209</v>
+      </c>
+      <c r="F41" s="16" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C42" s="15">
+        <v>45634</v>
+      </c>
+      <c r="D42" s="1">
+        <v>970</v>
+      </c>
+      <c r="E42" s="1">
+        <v>300</v>
+      </c>
+      <c r="F42" s="1">
+        <f>(D42-E42)</f>
+        <v>670</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" s="17" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="B44" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="C44" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="D44" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="E44" s="16" t="s">
+        <v>209</v>
+      </c>
+      <c r="F44" s="16" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C45" s="21">
+        <v>45682</v>
+      </c>
+      <c r="D45" s="1">
+        <v>670</v>
+      </c>
+      <c r="E45" s="1">
+        <v>200</v>
+      </c>
+      <c r="F45" s="1">
+        <f>(D45-E45)</f>
+        <v>470</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" s="17" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="B47" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="C47" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="D47" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="E47" s="16" t="s">
+        <v>209</v>
+      </c>
+      <c r="F47" s="16" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C48" s="15">
+        <v>45690</v>
+      </c>
+      <c r="D48" s="1">
+        <v>470</v>
+      </c>
+      <c r="E48" s="1">
+        <v>300</v>
+      </c>
+      <c r="F48" s="1">
+        <f>(D48-E48)</f>
+        <v>170</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="A49" s="17" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8">
+      <c r="A50" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="B50" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="C50" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="D50" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="E50" s="16" t="s">
+        <v>209</v>
+      </c>
+      <c r="F50" s="16" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8">
+      <c r="A51" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C51" s="15">
+        <v>45779</v>
+      </c>
+      <c r="D51" s="1">
+        <v>170</v>
+      </c>
+      <c r="E51" s="1">
+        <v>70</v>
+      </c>
+      <c r="F51" s="1">
+        <f>(D51-E51)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8">
+      <c r="A52" s="17" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8">
+      <c r="A53" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="B53" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="C53" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="D53" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="E53" s="16" t="s">
+        <v>209</v>
+      </c>
+      <c r="F53" s="16" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8">
+      <c r="A54" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C54" s="21">
+        <v>45932</v>
+      </c>
+      <c r="D54" s="1">
+        <v>70</v>
+      </c>
+      <c r="E54" s="1">
+        <v>30</v>
+      </c>
+      <c r="F54" s="1">
+        <f>(D54-E54)</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8">
+      <c r="A55" s="17" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8">
+      <c r="A56" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="B56" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="C56" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="D56" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="E56" s="16" t="s">
+        <v>209</v>
+      </c>
+      <c r="F56" s="16" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8">
+      <c r="A57" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C57" s="23" t="s">
+        <v>219</v>
+      </c>
+      <c r="D57" s="1">
+        <v>40</v>
+      </c>
+      <c r="E57" s="1">
+        <v>40</v>
+      </c>
+      <c r="F57" s="1">
+        <f>(D57-E57)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8">
+      <c r="F59" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8">
+      <c r="A60" s="19" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8">
+      <c r="A61" s="18" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8">
+      <c r="A62" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="B62" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="C62" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="D62" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="E62" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="F62" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="G62" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="H62" s="16" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8">
+      <c r="A63" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="E63" s="1">
+        <v>1000</v>
+      </c>
+      <c r="F63" s="1">
+        <v>2500</v>
+      </c>
+      <c r="G63" s="1">
+        <v>25</v>
+      </c>
+      <c r="H63" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF4210A9-9BC7-48DE-9A32-E3921EFE6C10}">
   <dimension ref="A1:F11"/>
@@ -2353,7 +4854,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D0B2F34-C77A-44EB-829F-BA8A4315E87C}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="G2" sqref="G2:G3"/>
     </sheetView>
   </sheetViews>
@@ -2455,8 +4956,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4BFA26D-5965-4F0E-B5D6-35562F52A7FB}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection sqref="A1:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>

</xml_diff>